<commit_message>
Add Travis CI and Generate badges
</commit_message>
<xml_diff>
--- a/input_data/data_errors_03/descricao.xlsx
+++ b/input_data/data_errors_03/descricao.xlsx
@@ -430,10 +430,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>

</xml_diff>